<commit_message>
add robot action (not complete yet)
</commit_message>
<xml_diff>
--- a/materials/新建 XLSX 工作表.xlsx
+++ b/materials/新建 XLSX 工作表.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="174">
   <si>
     <t>text</t>
   </si>
@@ -394,6 +394,9 @@
   </si>
   <si>
     <t>[S] 再来一局</t>
+  </si>
+  <si>
+    <t>抽并出了一张牌</t>
   </si>
   <si>
     <t>红0</t>
@@ -1703,8 +1706,8 @@
   <sheetPr/>
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="15" customHeight="1"/>
@@ -2459,9 +2462,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="82" customHeight="1" spans="1:1">
+    <row r="82" customHeight="1" spans="1:2">
       <c r="A82">
         <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2543,61 +2549,61 @@
     </row>
     <row r="2" customFormat="1" spans="1:19">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="O2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="P2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Q2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:19">
@@ -2661,61 +2667,61 @@
     </row>
     <row r="5" customFormat="1" spans="1:19">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="O5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="P5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Q5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="R5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="S5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" customFormat="1" spans="1:19">
@@ -2779,61 +2785,61 @@
     </row>
     <row r="8" customFormat="1" spans="1:19">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="O8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="P8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="Q8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="R8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="S8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="1:19">
@@ -2897,61 +2903,61 @@
     </row>
     <row r="11" customFormat="1" spans="1:19">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="O11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="P11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Q11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="R11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="S11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" ht="14.25"/>
@@ -2978,30 +2984,30 @@
         <v>198</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="1:9">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I14" s="8"/>
     </row>
@@ -3035,25 +3041,25 @@
     </row>
     <row r="17" customFormat="1" spans="1:9">
       <c r="A17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" t="s">
+        <v>145</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="B17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C17" t="s">
-        <v>143</v>
-      </c>
-      <c r="D17" t="s">
-        <v>143</v>
-      </c>
-      <c r="E17" t="s">
-        <v>144</v>
-      </c>
-      <c r="F17" t="s">
-        <v>144</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="I17" s="8"/>
     </row>
@@ -3087,25 +3093,25 @@
     </row>
     <row r="20" customFormat="1" spans="1:9">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E20" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F20" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I20" s="8"/>
     </row>
@@ -3139,25 +3145,25 @@
     </row>
     <row r="23" customFormat="1" ht="14.25" spans="1:9">
       <c r="A23" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B23" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I23" s="9"/>
     </row>
@@ -3189,28 +3195,28 @@
     </row>
     <row r="26" customFormat="1" spans="1:8">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E26" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F26" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G26" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H26" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3236,13 +3242,13 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F1">
         <v>118</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="6:8">
@@ -3250,12 +3256,12 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F3">
         <v>15</v>
@@ -3266,45 +3272,45 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F4">
         <f>F1-F2*F3</f>
         <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F5">
         <f>F4/(F2+1)</f>
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="8:12">
@@ -3326,18 +3332,18 @@
     </row>
     <row r="9" spans="3:8">
       <c r="C9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -3345,10 +3351,10 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -3356,10 +3362,10 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H12">
         <v>3</v>
@@ -3367,10 +3373,10 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H13">
         <v>4</v>
@@ -3378,10 +3384,10 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C14" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H14">
         <v>5</v>
@@ -3389,7 +3395,7 @@
     </row>
     <row r="15" spans="3:8">
       <c r="C15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H15">
         <v>6</v>
@@ -3402,7 +3408,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H17">
         <v>8</v>
@@ -3410,7 +3416,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H18">
         <v>9</v>
@@ -3418,7 +3424,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H19">
         <v>10</v>
@@ -3426,7 +3432,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H20">
         <v>11</v>
@@ -3434,7 +3440,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H21">
         <v>12</v>
@@ -3447,7 +3453,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H23">
         <v>14</v>
@@ -3455,47 +3461,47 @@
     </row>
     <row r="24" spans="2:8">
       <c r="B24" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H26" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I26" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H28" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>